<commit_message>
Simplify unnecessarily long PV names
</commit_message>
<xml_diff>
--- a/etc/Delta_v2.xlsx
+++ b/etc/Delta_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Ondulador\etherip-ioc\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="536" documentId="13_ncr:1_{6378EC21-B70E-45CA-8FBF-B3322DB496BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21EBF05A-953C-4209-BFD8-7C71F4F3BFD4}"/>
+  <xr:revisionPtr revIDLastSave="632" documentId="13_ncr:1_{6378EC21-B70E-45CA-8FBF-B3322DB496BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59BC9397-F5B9-4189-8218-894221DBA26B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="5" r:id="rId1"/>
@@ -477,7 +477,7 @@
     <t>Actual pos virtual CID mod 01</t>
   </si>
   <si>
-    <t>VirtCIDActualPos</t>
+    <t>CIDVirtPos</t>
   </si>
   <si>
     <t>CID1_PTH.ActualPosition</t>
@@ -486,7 +486,7 @@
     <t>Actual pos virtual CIE mod 01</t>
   </si>
   <si>
-    <t>VirtCIEActualPos</t>
+    <t>CIEVirtPos</t>
   </si>
   <si>
     <t>CIE1_PTH.ActualPosition</t>
@@ -495,7 +495,7 @@
     <t>Actual pos virtual CSD mod 01</t>
   </si>
   <si>
-    <t>VirtCSDActualPos</t>
+    <t>CSDVirtPos</t>
   </si>
   <si>
     <t>CSD1_PTH.ActualPosition</t>
@@ -504,7 +504,7 @@
     <t>Actual pos virtual CSE mod 01</t>
   </si>
   <si>
-    <t>VirtCSEActualPos</t>
+    <t>CSEVirtPos</t>
   </si>
   <si>
     <t>CSE1_PTH.ActualPosition</t>
@@ -513,7 +513,7 @@
     <t>Actual velocity virtual CID mod 01</t>
   </si>
   <si>
-    <t>VirtCIDActualVelo</t>
+    <t>CIDVirtVelo</t>
   </si>
   <si>
     <t>CID1_PTH.ActualVelocity</t>
@@ -522,7 +522,7 @@
     <t>Actual velocity virtual CIE mod 01</t>
   </si>
   <si>
-    <t>VirtCIEActualVelo</t>
+    <t>CIEVirtVelo</t>
   </si>
   <si>
     <t>CIE1_PTH.ActualVelocity</t>
@@ -531,7 +531,7 @@
     <t>Actual velocity virtual CSD mod 01</t>
   </si>
   <si>
-    <t>VirtCSDActualVelo</t>
+    <t>CSDVirtVelo</t>
   </si>
   <si>
     <t>CSD1_PTH.ActualVelocity</t>
@@ -540,7 +540,7 @@
     <t>Actual velocity virtual CSE mod 01</t>
   </si>
   <si>
-    <t>VirtCSEActualVelo</t>
+    <t>CSEVirtVelo</t>
   </si>
   <si>
     <t>CSE1_PTH.ActualVelocity</t>
@@ -549,7 +549,7 @@
     <t>Actual position physical CID mod 01</t>
   </si>
   <si>
-    <t>PhyCIDActualPos</t>
+    <t>CIDPhyPos</t>
   </si>
   <si>
     <t>CID1_PHY.ActualPosition</t>
@@ -558,7 +558,7 @@
     <t>Actual position physical CIE mod 01</t>
   </si>
   <si>
-    <t>PhyCIEActualPos</t>
+    <t>CIEPhyPos</t>
   </si>
   <si>
     <t>CIE1_PHY.ActualPosition</t>
@@ -567,7 +567,7 @@
     <t>Actual position physical CSD mod 01</t>
   </si>
   <si>
-    <t>PhyCSDActualPos</t>
+    <t>CSDPhyPos</t>
   </si>
   <si>
     <t>CSD1_PHY.ActualPosition</t>
@@ -576,7 +576,7 @@
     <t>Actual position physical CSE mod 01</t>
   </si>
   <si>
-    <t>PhyCSEActualPos</t>
+    <t>CSEPhyPos</t>
   </si>
   <si>
     <t>CSE1_PHY.ActualPosition</t>
@@ -585,7 +585,7 @@
     <t>Actual velocity physical CID mod 01</t>
   </si>
   <si>
-    <t>PhyCIDActualVelo</t>
+    <t>CIDPhyVelo</t>
   </si>
   <si>
     <t>CID1_PHY.ActualVelocity</t>
@@ -594,7 +594,7 @@
     <t>Actual velocity physical CIE mod 01</t>
   </si>
   <si>
-    <t>PhyCIEActualVelo</t>
+    <t>CIEPhyVelo</t>
   </si>
   <si>
     <t>CIE1_PHY.ActualVelocity</t>
@@ -603,7 +603,7 @@
     <t>Actual velocity physical CSD mod 01</t>
   </si>
   <si>
-    <t>PhyCSDActualVelo</t>
+    <t>CSDPhyVelo</t>
   </si>
   <si>
     <t>CSD1_PHY.ActualVelocity</t>
@@ -612,7 +612,7 @@
     <t>Actual velocity physical CSE mod 01</t>
   </si>
   <si>
-    <t>PhyCSEActualVelo</t>
+    <t>CSEPhyVelo</t>
   </si>
   <si>
     <t>CSE1_PHY.ActualVelocity</t>
@@ -2146,14 +2146,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2165,22 +2165,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2207,16 +2207,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2225,22 +2225,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9026,7 +9026,7 @@
       </c>
       <c r="F29" s="9" t="str">
         <f>C29&amp;D29&amp;E29</f>
-        <v>$(PREFIX_MOD01)VirtCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CIDVirtPos-Mon</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>121</v>
@@ -9078,7 +9078,7 @@
       </c>
       <c r="F30" s="9" t="str">
         <f>C30&amp;D30&amp;E30</f>
-        <v>$(PREFIX_MOD01)VirtCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CIEVirtPos-Mon</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>121</v>
@@ -9130,7 +9130,7 @@
       </c>
       <c r="F31" s="9" t="str">
         <f>C31&amp;D31&amp;E31</f>
-        <v>$(PREFIX_MOD01)VirtCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CSDVirtPos-Mon</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>121</v>
@@ -9182,7 +9182,7 @@
       </c>
       <c r="F32" s="9" t="str">
         <f>C32&amp;D32&amp;E32</f>
-        <v>$(PREFIX_MOD01)VirtCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CSEVirtPos-Mon</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>121</v>
@@ -9234,7 +9234,7 @@
       </c>
       <c r="F33" s="9" t="str">
         <f>C33&amp;D33&amp;E33</f>
-        <v>$(PREFIX_MOD01)VirtCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CIDVirtVelo-Mon</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>121</v>
@@ -9286,7 +9286,7 @@
       </c>
       <c r="F34" s="9" t="str">
         <f>C34&amp;D34&amp;E34</f>
-        <v>$(PREFIX_MOD01)VirtCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CIEVirtVelo-Mon</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>121</v>
@@ -9338,7 +9338,7 @@
       </c>
       <c r="F35" s="9" t="str">
         <f>C35&amp;D35&amp;E35</f>
-        <v>$(PREFIX_MOD01)VirtCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CSDVirtVelo-Mon</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>121</v>
@@ -9390,7 +9390,7 @@
       </c>
       <c r="F36" s="9" t="str">
         <f>C36&amp;D36&amp;E36</f>
-        <v>$(PREFIX_MOD01)VirtCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CSEVirtVelo-Mon</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>121</v>
@@ -9442,7 +9442,7 @@
       </c>
       <c r="F37" s="9" t="str">
         <f>C37&amp;D37&amp;E37</f>
-        <v>$(PREFIX_MOD01)PhyCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CIDPhyPos-Mon</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>121</v>
@@ -9494,7 +9494,7 @@
       </c>
       <c r="F38" s="9" t="str">
         <f>C38&amp;D38&amp;E38</f>
-        <v>$(PREFIX_MOD01)PhyCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CIEPhyPos-Mon</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>121</v>
@@ -9546,7 +9546,7 @@
       </c>
       <c r="F39" s="9" t="str">
         <f>C39&amp;D39&amp;E39</f>
-        <v>$(PREFIX_MOD01)PhyCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CSDPhyPos-Mon</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>121</v>
@@ -9598,7 +9598,7 @@
       </c>
       <c r="F40" s="9" t="str">
         <f>C40&amp;D40&amp;E40</f>
-        <v>$(PREFIX_MOD01)PhyCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD01)CSEPhyPos-Mon</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>121</v>
@@ -9650,7 +9650,7 @@
       </c>
       <c r="F41" s="9" t="str">
         <f>C41&amp;D41&amp;E41</f>
-        <v>$(PREFIX_MOD01)PhyCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CIDPhyVelo-Mon</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>121</v>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="F42" s="9" t="str">
         <f>C42&amp;D42&amp;E42</f>
-        <v>$(PREFIX_MOD01)PhyCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CIEPhyVelo-Mon</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>121</v>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="F43" s="9" t="str">
         <f>C43&amp;D43&amp;E43</f>
-        <v>$(PREFIX_MOD01)PhyCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CSDPhyVelo-Mon</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>121</v>
@@ -9806,7 +9806,7 @@
       </c>
       <c r="F44" s="9" t="str">
         <f>C44&amp;D44&amp;E44</f>
-        <v>$(PREFIX_MOD01)PhyCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD01)CSEPhyVelo-Mon</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>121</v>
@@ -13554,7 +13554,7 @@
       </c>
       <c r="F29" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CIDVirtPos-Mon</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>121</v>
@@ -13606,7 +13606,7 @@
       </c>
       <c r="F30" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CIEVirtPos-Mon</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>121</v>
@@ -13658,7 +13658,7 @@
       </c>
       <c r="F31" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CSDVirtPos-Mon</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>121</v>
@@ -13710,7 +13710,7 @@
       </c>
       <c r="F32" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CSEVirtPos-Mon</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>121</v>
@@ -13762,7 +13762,7 @@
       </c>
       <c r="F33" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CIDVirtVelo-Mon</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>121</v>
@@ -13814,7 +13814,7 @@
       </c>
       <c r="F34" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CIEVirtVelo-Mon</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>121</v>
@@ -13866,7 +13866,7 @@
       </c>
       <c r="F35" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CSDVirtVelo-Mon</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>121</v>
@@ -13918,7 +13918,7 @@
       </c>
       <c r="F36" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)VirtCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CSEVirtVelo-Mon</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>121</v>
@@ -13970,7 +13970,7 @@
       </c>
       <c r="F37" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CIDPhyPos-Mon</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>121</v>
@@ -14022,7 +14022,7 @@
       </c>
       <c r="F38" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CIEPhyPos-Mon</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>121</v>
@@ -14074,7 +14074,7 @@
       </c>
       <c r="F39" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CSDPhyPos-Mon</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>121</v>
@@ -14126,7 +14126,7 @@
       </c>
       <c r="F40" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD02)CSEPhyPos-Mon</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>121</v>
@@ -14178,7 +14178,7 @@
       </c>
       <c r="F41" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CIDPhyVelo-Mon</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>121</v>
@@ -14230,7 +14230,7 @@
       </c>
       <c r="F42" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CIEPhyVelo-Mon</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>121</v>
@@ -14282,7 +14282,7 @@
       </c>
       <c r="F43" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CSDPhyVelo-Mon</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>121</v>
@@ -14334,7 +14334,7 @@
       </c>
       <c r="F44" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD02)PhyCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD02)CSEPhyVelo-Mon</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>121</v>
@@ -18027,7 +18027,7 @@
       </c>
       <c r="F29" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CIDVirtPos-Mon</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>121</v>
@@ -18079,7 +18079,7 @@
       </c>
       <c r="F30" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CIEVirtPos-Mon</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>121</v>
@@ -18131,7 +18131,7 @@
       </c>
       <c r="F31" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CSDVirtPos-Mon</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>121</v>
@@ -18183,7 +18183,7 @@
       </c>
       <c r="F32" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CSEVirtPos-Mon</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>121</v>
@@ -18235,7 +18235,7 @@
       </c>
       <c r="F33" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CIDVirtVelo-Mon</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>121</v>
@@ -18287,7 +18287,7 @@
       </c>
       <c r="F34" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CIEVirtVelo-Mon</v>
       </c>
       <c r="G34" s="11" t="s">
         <v>121</v>
@@ -18339,7 +18339,7 @@
       </c>
       <c r="F35" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CSDVirtVelo-Mon</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>121</v>
@@ -18391,7 +18391,7 @@
       </c>
       <c r="F36" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)VirtCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CSEVirtVelo-Mon</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>121</v>
@@ -18443,7 +18443,7 @@
       </c>
       <c r="F37" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCIDActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CIDPhyPos-Mon</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>121</v>
@@ -18495,7 +18495,7 @@
       </c>
       <c r="F38" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCIEActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CIEPhyPos-Mon</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>121</v>
@@ -18547,7 +18547,7 @@
       </c>
       <c r="F39" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCSDActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CSDPhyPos-Mon</v>
       </c>
       <c r="G39" s="11" t="s">
         <v>121</v>
@@ -18599,7 +18599,7 @@
       </c>
       <c r="F40" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCSEActualPos-Mon</v>
+        <v>$(PREFIX_MOD03)CSEPhyPos-Mon</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>121</v>
@@ -18651,7 +18651,7 @@
       </c>
       <c r="F41" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCIDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CIDPhyVelo-Mon</v>
       </c>
       <c r="G41" s="10" t="s">
         <v>121</v>
@@ -18703,7 +18703,7 @@
       </c>
       <c r="F42" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCIEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CIEPhyVelo-Mon</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>121</v>
@@ -18755,7 +18755,7 @@
       </c>
       <c r="F43" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCSDActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CSDPhyVelo-Mon</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>121</v>
@@ -18807,7 +18807,7 @@
       </c>
       <c r="F44" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>$(PREFIX_MOD03)PhyCSEActualVelo-Mon</v>
+        <v>$(PREFIX_MOD03)CSEPhyVelo-Mon</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Fix module motion state PV fields
Fix fields of motion state PV of each module: <Module Prefix>MotionState-Mon

Instead of {0: Moving| 1: Done}, enum fields should be {0: Ready, 1: Moving, 2: Done}.
</commit_message>
<xml_diff>
--- a/etc/Delta_v2.xlsx
+++ b/etc/Delta_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2418" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="586">
   <si>
     <t xml:space="preserve">Nº</t>
   </si>
@@ -283,6 +283,9 @@
     <t xml:space="preserve">ER_Mov_Stat_Mod_01</t>
   </si>
   <si>
+    <t xml:space="preserve">Ready</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moving</t>
   </si>
   <si>
@@ -296,9 +299,6 @@
   </si>
   <si>
     <t xml:space="preserve">ER_Mov_Stat_Mod_01_Axis_CID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ready</t>
   </si>
   <si>
     <t xml:space="preserve">Module 01 CIE motion status</t>
@@ -3051,8 +3051,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F56" activeCellId="0" sqref="F56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3492,7 +3492,7 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>7</v>
       </c>
@@ -3536,7 +3536,9 @@
       <c r="P8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="17"/>
+      <c r="Q8" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -3551,13 +3553,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>76</v>
@@ -3574,7 +3576,7 @@
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>32</v>
@@ -3585,13 +3587,13 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -3641,13 +3643,13 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
@@ -3697,13 +3699,13 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
@@ -3753,13 +3755,13 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
@@ -7386,8 +7388,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B81" activeCellId="0" sqref="B81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7826,7 +7828,7 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>7</v>
       </c>
@@ -7870,7 +7872,9 @@
       <c r="P8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="17"/>
+      <c r="Q8" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -7891,7 +7895,7 @@
         <v>301</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>76</v>
@@ -7919,13 +7923,13 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -7975,13 +7979,13 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P10" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
@@ -8031,13 +8035,13 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
@@ -8087,13 +8091,13 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
@@ -11665,8 +11669,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B83" activeCellId="0" sqref="B83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12105,7 +12109,7 @@
       <c r="X7" s="17"/>
       <c r="Y7" s="17"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>7</v>
       </c>
@@ -12149,7 +12153,9 @@
       <c r="P8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="Q8" s="17"/>
+      <c r="Q8" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="R8" s="17"/>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -12170,7 +12176,7 @@
         <v>444</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>76</v>
@@ -12198,13 +12204,13 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
       <c r="O9" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P9" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
@@ -12254,13 +12260,13 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R10" s="34"/>
       <c r="S10" s="17"/>
@@ -12310,13 +12316,13 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
@@ -12366,13 +12372,13 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>

</xml_diff>

<commit_message>
delta: Change *TorqueRef* PV names
Replace *TorqueRef* by *Torque* in PV names that contain
this substring to avoid conflict with features that are
being developed and that will use the "Ref" substring
to indicate when a PV value is a reference for comparison
with the value of some related PVs.
</commit_message>
<xml_diff>
--- a/etc/Delta_v2.xlsx
+++ b/etc/Delta_v2.xlsx
@@ -682,7 +682,7 @@
     <t xml:space="preserve">Torque reference CID mod 01</t>
   </si>
   <si>
-    <t xml:space="preserve">CIDTorqueRef</t>
+    <t xml:space="preserve">CIDTorque</t>
   </si>
   <si>
     <t xml:space="preserve">%</t>
@@ -694,7 +694,7 @@
     <t xml:space="preserve">Torque reference CIE mod 01</t>
   </si>
   <si>
-    <t xml:space="preserve">CIETorqueRef</t>
+    <t xml:space="preserve">CIETorque</t>
   </si>
   <si>
     <t xml:space="preserve">CIE1_PHY.TorqueReference</t>
@@ -703,7 +703,7 @@
     <t xml:space="preserve">Torque reference CSD mod 01</t>
   </si>
   <si>
-    <t xml:space="preserve">CSDTorqueRef</t>
+    <t xml:space="preserve">CSDTorque</t>
   </si>
   <si>
     <t xml:space="preserve">CSD1_PHY.TorqueReference</t>
@@ -712,7 +712,7 @@
     <t xml:space="preserve">Torque reference CSE mod 01</t>
   </si>
   <si>
-    <t xml:space="preserve">CSETorqueRef</t>
+    <t xml:space="preserve">CSETorque</t>
   </si>
   <si>
     <t xml:space="preserve">CSE1_PHY.TorqueReference</t>
@@ -3051,8 +3051,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5900,7 +5900,7 @@
       </c>
       <c r="F53" s="13" t="str">
         <f aca="false">C53&amp;D53&amp;E53</f>
-        <v>$(PREFIX_MOD01)CIDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD01)CIDTorque-Mon</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>121</v>
@@ -5952,7 +5952,7 @@
       </c>
       <c r="F54" s="13" t="str">
         <f aca="false">C54&amp;D54&amp;E54</f>
-        <v>$(PREFIX_MOD01)CIETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD01)CIETorque-Mon</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>121</v>
@@ -6004,7 +6004,7 @@
       </c>
       <c r="F55" s="13" t="str">
         <f aca="false">C55&amp;D55&amp;E55</f>
-        <v>$(PREFIX_MOD01)CSDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD01)CSDTorque-Mon</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>121</v>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="F56" s="13" t="str">
         <f aca="false">C56&amp;D56&amp;E56</f>
-        <v>$(PREFIX_MOD01)CSETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD01)CSETorque-Mon</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>121</v>
@@ -7388,8 +7388,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10236,7 +10236,7 @@
       </c>
       <c r="F53" s="13" t="str">
         <f aca="false">C53&amp;D53&amp;E53</f>
-        <v>$(PREFIX_MOD02)CIDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD02)CIDTorque-Mon</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>121</v>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="F54" s="13" t="str">
         <f aca="false">C54&amp;D54&amp;E54</f>
-        <v>$(PREFIX_MOD02)CIETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD02)CIETorque-Mon</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>121</v>
@@ -10340,7 +10340,7 @@
       </c>
       <c r="F55" s="13" t="str">
         <f aca="false">C55&amp;D55&amp;E55</f>
-        <v>$(PREFIX_MOD02)CSDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD02)CSDTorque-Mon</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>121</v>
@@ -10392,7 +10392,7 @@
       </c>
       <c r="F56" s="13" t="str">
         <f aca="false">C56&amp;D56&amp;E56</f>
-        <v>$(PREFIX_MOD02)CSETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD02)CSETorque-Mon</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>121</v>
@@ -11669,8 +11669,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14517,7 +14517,7 @@
       </c>
       <c r="F53" s="13" t="str">
         <f aca="false">C53&amp;D53&amp;E53</f>
-        <v>$(PREFIX_MOD03)CIDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD03)CIDTorque-Mon</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>121</v>
@@ -14569,7 +14569,7 @@
       </c>
       <c r="F54" s="13" t="str">
         <f aca="false">C54&amp;D54&amp;E54</f>
-        <v>$(PREFIX_MOD03)CIETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD03)CIETorque-Mon</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>121</v>
@@ -14621,7 +14621,7 @@
       </c>
       <c r="F55" s="13" t="str">
         <f aca="false">C55&amp;D55&amp;E55</f>
-        <v>$(PREFIX_MOD03)CSDTorqueRef-Mon</v>
+        <v>$(PREFIX_MOD03)CSDTorque-Mon</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>121</v>
@@ -14673,7 +14673,7 @@
       </c>
       <c r="F56" s="13" t="str">
         <f aca="false">C56&amp;D56&amp;E56</f>
-        <v>$(PREFIX_MOD03)CSETorqueRef-Mon</v>
+        <v>$(PREFIX_MOD03)CSETorque-Mon</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Add motor temperature PVs to delta spreadsheet
</commit_message>
<xml_diff>
--- a/etc/Delta_v2.xlsx
+++ b/etc/Delta_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrei.pereira\Documents\Delta\etherip-ioc\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF315722-5CEC-4316-B67C-2CD327FA7E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6990324E-4DA0-41B2-9FFC-94F7CEF58792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="630">
   <si>
     <t>Nº</t>
   </si>
@@ -1842,6 +1842,93 @@
   </si>
   <si>
     <t>ER_Conf_Dec_Mod_03</t>
+  </si>
+  <si>
+    <t>Motor temperature CID mod 01</t>
+  </si>
+  <si>
+    <t>CIDMtrTemp</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_01_Axis_CID</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>Motor temperature CIE mod 01</t>
+  </si>
+  <si>
+    <t>CIEMtrTemp</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_01_Axis_CIE</t>
+  </si>
+  <si>
+    <t>Motor temperature CSD mod 01</t>
+  </si>
+  <si>
+    <t>CSDMtrTemp</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_01_Axis_CSD</t>
+  </si>
+  <si>
+    <t>Motor temperature CSE mod 01</t>
+  </si>
+  <si>
+    <t>CSEMtrTemp</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_01_Axis_CSE</t>
+  </si>
+  <si>
+    <t>Motor temperature CID mod 02</t>
+  </si>
+  <si>
+    <t>Motor temperature CIE mod 02</t>
+  </si>
+  <si>
+    <t>Motor temperature CSD mod 02</t>
+  </si>
+  <si>
+    <t>Motor temperature CSE mod 02</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_02_Axis_CID</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_02_Axis_CIE</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_02_Axis_CSD</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_02_Axis_CSE</t>
+  </si>
+  <si>
+    <t>Motor temperature CID mod 03</t>
+  </si>
+  <si>
+    <t>Motor temperature CIE mod 03</t>
+  </si>
+  <si>
+    <t>Motor temperature CSD mod 03</t>
+  </si>
+  <si>
+    <t>Motor temperature CSE mod 03</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_03_Axis_CID</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_03_Axis_CIE</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_03_Axis_CSD</t>
+  </si>
+  <si>
+    <t>ER_Motor_Temperature_Mod_03_Axis_CSE</t>
   </si>
 </sst>
 </file>
@@ -2735,8 +2822,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela1" displayName="Tabela1" ref="A1:Y79" totalsRowShown="0">
-  <autoFilter ref="A1:Y79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela1" displayName="Tabela1" ref="A1:Y83" totalsRowShown="0">
+  <autoFilter ref="A1:Y83" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nº"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description"/>
@@ -2769,8 +2856,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela2" displayName="Tabela2" ref="A1:Y79" totalsRowShown="0">
-  <autoFilter ref="A1:Y79" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabela2" displayName="Tabela2" ref="A1:Y83" totalsRowShown="0">
+  <autoFilter ref="A1:Y83" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Nº"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Description"/>
@@ -3135,7 +3222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -3144,7 +3231,7 @@
     <col min="2" max="2" width="37.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="30.26953125" customWidth="1"/>
+    <col min="6" max="6" width="32.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.453125" customWidth="1"/>
     <col min="8" max="8" width="9.453125" customWidth="1"/>
     <col min="10" max="10" width="22.81640625" customWidth="1"/>
@@ -3379,10 +3466,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y79"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3394,7 +3481,8 @@
     <col min="6" max="6" width="39.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.453125" customWidth="1"/>
     <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="10" max="10" width="37.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.54296875" customWidth="1"/>
     <col min="14" max="14" width="10.26953125" customWidth="1"/>
     <col min="15" max="15" width="10.08984375" customWidth="1"/>
@@ -6905,7 +6993,7 @@
         <v>76</v>
       </c>
       <c r="F66" s="23" t="str">
-        <f t="shared" ref="F66:F97" si="2">C66&amp;D66&amp;E66</f>
+        <f t="shared" ref="F66:F79" si="2">C66&amp;D66&amp;E66</f>
         <v>$(PREFIX_MOD01)CIEPosLimSw-Mon</v>
       </c>
       <c r="G66" s="24" t="s">
@@ -7611,6 +7699,214 @@
       <c r="W79" s="27"/>
       <c r="X79" s="27"/>
       <c r="Y79" s="27"/>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A80" s="8">
+        <v>79</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F80" s="23" t="str">
+        <f t="shared" ref="F80" si="3">C80&amp;D80&amp;E80</f>
+        <v>$(PREFIX_MOD01)CIDMtrTemp-Mon</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H80" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I80" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J80" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="K80" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="24">
+        <v>1</v>
+      </c>
+      <c r="M80" s="27"/>
+      <c r="N80" s="27"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="27"/>
+      <c r="Q80" s="27"/>
+      <c r="R80" s="27"/>
+      <c r="S80" s="27"/>
+      <c r="T80" s="27"/>
+      <c r="U80" s="27"/>
+      <c r="V80" s="27"/>
+      <c r="W80" s="27"/>
+      <c r="X80" s="27"/>
+      <c r="Y80" s="27"/>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A81" s="18">
+        <v>80</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>606</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F81" s="23" t="str">
+        <f t="shared" ref="F81" si="4">C81&amp;D81&amp;E81</f>
+        <v>$(PREFIX_MOD01)CIEMtrTemp-Mon</v>
+      </c>
+      <c r="G81" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H81" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I81" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J81" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="K81" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="24">
+        <v>1</v>
+      </c>
+      <c r="M81" s="27"/>
+      <c r="N81" s="27"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="27"/>
+      <c r="Q81" s="27"/>
+      <c r="R81" s="27"/>
+      <c r="S81" s="27"/>
+      <c r="T81" s="27"/>
+      <c r="U81" s="27"/>
+      <c r="V81" s="27"/>
+      <c r="W81" s="27"/>
+      <c r="X81" s="27"/>
+      <c r="Y81" s="27"/>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A82" s="18">
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>608</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F82" s="23" t="str">
+        <f t="shared" ref="F82" si="5">C82&amp;D82&amp;E82</f>
+        <v>$(PREFIX_MOD01)CSDMtrTemp-Mon</v>
+      </c>
+      <c r="G82" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H82" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I82" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J82" s="24" t="s">
+        <v>610</v>
+      </c>
+      <c r="K82" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="24">
+        <v>1</v>
+      </c>
+      <c r="M82" s="27"/>
+      <c r="N82" s="27"/>
+      <c r="O82" s="27"/>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="27"/>
+      <c r="R82" s="27"/>
+      <c r="S82" s="27"/>
+      <c r="T82" s="27"/>
+      <c r="U82" s="27"/>
+      <c r="V82" s="27"/>
+      <c r="W82" s="27"/>
+      <c r="X82" s="27"/>
+      <c r="Y82" s="27"/>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A83" s="18">
+        <v>82</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F83" s="23" t="str">
+        <f t="shared" ref="F83" si="6">C83&amp;D83&amp;E83</f>
+        <v>$(PREFIX_MOD01)CSEMtrTemp-Mon</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I83" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J83" s="24" t="s">
+        <v>613</v>
+      </c>
+      <c r="K83" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L83" s="24">
+        <v>1</v>
+      </c>
+      <c r="M83" s="27"/>
+      <c r="N83" s="27"/>
+      <c r="O83" s="27"/>
+      <c r="P83" s="27"/>
+      <c r="Q83" s="27"/>
+      <c r="R83" s="27"/>
+      <c r="S83" s="27"/>
+      <c r="T83" s="27"/>
+      <c r="U83" s="27"/>
+      <c r="V83" s="27"/>
+      <c r="W83" s="27"/>
+      <c r="X83" s="27"/>
+      <c r="Y83" s="27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B19:B32">
@@ -7689,7 +7985,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E79" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E83" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"-Mon,-Sel,-Sts,-SP,-RB,-Cmd"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7704,10 +8000,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y79"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7718,7 +8014,7 @@
     <col min="6" max="6" width="39.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.453125" customWidth="1"/>
     <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="10" max="10" width="37.54296875" customWidth="1"/>
+    <col min="10" max="10" width="41.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.54296875" customWidth="1"/>
     <col min="14" max="14" width="10.26953125" customWidth="1"/>
     <col min="15" max="15" width="10.08984375" customWidth="1"/>
@@ -11229,7 +11525,7 @@
         <v>76</v>
       </c>
       <c r="F66" s="23" t="str">
-        <f t="shared" ref="F66:F97" si="2">C66&amp;D66&amp;E66</f>
+        <f t="shared" ref="F66:F83" si="2">C66&amp;D66&amp;E66</f>
         <v>$(PREFIX_MOD02)CIEPosLimSw-Mon</v>
       </c>
       <c r="G66" s="24" t="s">
@@ -11935,6 +12231,214 @@
       <c r="W79" s="17"/>
       <c r="X79" s="17"/>
       <c r="Y79" s="17"/>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A80" s="8">
+        <v>79</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F80" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD02)CIDMtrTemp-Mon</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H80" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I80" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J80" s="24" t="s">
+        <v>618</v>
+      </c>
+      <c r="K80" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="24">
+        <v>1</v>
+      </c>
+      <c r="M80" s="27"/>
+      <c r="N80" s="27"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="27"/>
+      <c r="Q80" s="27"/>
+      <c r="R80" s="27"/>
+      <c r="S80" s="27"/>
+      <c r="T80" s="27"/>
+      <c r="U80" s="27"/>
+      <c r="V80" s="27"/>
+      <c r="W80" s="27"/>
+      <c r="X80" s="27"/>
+      <c r="Y80" s="27"/>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A81" s="18">
+        <v>80</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>615</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>606</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F81" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD02)CIEMtrTemp-Mon</v>
+      </c>
+      <c r="G81" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H81" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I81" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J81" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="K81" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="24">
+        <v>1</v>
+      </c>
+      <c r="M81" s="27"/>
+      <c r="N81" s="27"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="27"/>
+      <c r="Q81" s="27"/>
+      <c r="R81" s="27"/>
+      <c r="S81" s="27"/>
+      <c r="T81" s="27"/>
+      <c r="U81" s="27"/>
+      <c r="V81" s="27"/>
+      <c r="W81" s="27"/>
+      <c r="X81" s="27"/>
+      <c r="Y81" s="27"/>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A82" s="18">
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F82" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD02)CSDMtrTemp-Mon</v>
+      </c>
+      <c r="G82" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H82" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I82" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J82" s="24" t="s">
+        <v>620</v>
+      </c>
+      <c r="K82" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="24">
+        <v>1</v>
+      </c>
+      <c r="M82" s="27"/>
+      <c r="N82" s="27"/>
+      <c r="O82" s="27"/>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="27"/>
+      <c r="R82" s="27"/>
+      <c r="S82" s="27"/>
+      <c r="T82" s="27"/>
+      <c r="U82" s="27"/>
+      <c r="V82" s="27"/>
+      <c r="W82" s="27"/>
+      <c r="X82" s="27"/>
+      <c r="Y82" s="27"/>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A83" s="18">
+        <v>82</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>617</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F83" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD02)CSEMtrTemp-Mon</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I83" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J83" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="K83" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L83" s="24">
+        <v>1</v>
+      </c>
+      <c r="M83" s="27"/>
+      <c r="N83" s="27"/>
+      <c r="O83" s="27"/>
+      <c r="P83" s="27"/>
+      <c r="Q83" s="27"/>
+      <c r="R83" s="27"/>
+      <c r="S83" s="27"/>
+      <c r="T83" s="27"/>
+      <c r="U83" s="27"/>
+      <c r="V83" s="27"/>
+      <c r="W83" s="27"/>
+      <c r="X83" s="27"/>
+      <c r="Y83" s="27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B19:B32">
@@ -11958,7 +12462,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E79" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E83" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"-Mon,-Sel,-Sts,-SP,-RB,-Cmd"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11973,10 +12477,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Y79"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11987,7 +12491,7 @@
     <col min="6" max="6" width="39.08984375" customWidth="1"/>
     <col min="7" max="7" width="12.453125" customWidth="1"/>
     <col min="8" max="8" width="9.453125" customWidth="1"/>
-    <col min="10" max="10" width="37.54296875" customWidth="1"/>
+    <col min="10" max="10" width="41.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.54296875" customWidth="1"/>
     <col min="14" max="14" width="10.26953125" customWidth="1"/>
     <col min="15" max="15" width="10.08984375" customWidth="1"/>
@@ -15498,7 +16002,7 @@
         <v>76</v>
       </c>
       <c r="F66" s="23" t="str">
-        <f t="shared" ref="F66:F97" si="2">C66&amp;D66&amp;E66</f>
+        <f t="shared" ref="F66:F83" si="2">C66&amp;D66&amp;E66</f>
         <v>$(PREFIX_MOD03)CIEPosLimSw-Mon</v>
       </c>
       <c r="G66" s="24" t="s">
@@ -16204,6 +16708,214 @@
       <c r="W79" s="17"/>
       <c r="X79" s="17"/>
       <c r="Y79" s="17"/>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A80" s="8">
+        <v>79</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>622</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F80" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD03)CIDMtrTemp-Mon</v>
+      </c>
+      <c r="G80" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H80" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I80" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J80" s="24" t="s">
+        <v>626</v>
+      </c>
+      <c r="K80" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" s="24">
+        <v>1</v>
+      </c>
+      <c r="M80" s="27"/>
+      <c r="N80" s="27"/>
+      <c r="O80" s="27"/>
+      <c r="P80" s="27"/>
+      <c r="Q80" s="27"/>
+      <c r="R80" s="27"/>
+      <c r="S80" s="27"/>
+      <c r="T80" s="27"/>
+      <c r="U80" s="27"/>
+      <c r="V80" s="27"/>
+      <c r="W80" s="27"/>
+      <c r="X80" s="27"/>
+      <c r="Y80" s="27"/>
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A81" s="18">
+        <v>80</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>606</v>
+      </c>
+      <c r="E81" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F81" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD03)CIEMtrTemp-Mon</v>
+      </c>
+      <c r="G81" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H81" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I81" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J81" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="K81" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81" s="24">
+        <v>1</v>
+      </c>
+      <c r="M81" s="27"/>
+      <c r="N81" s="27"/>
+      <c r="O81" s="27"/>
+      <c r="P81" s="27"/>
+      <c r="Q81" s="27"/>
+      <c r="R81" s="27"/>
+      <c r="S81" s="27"/>
+      <c r="T81" s="27"/>
+      <c r="U81" s="27"/>
+      <c r="V81" s="27"/>
+      <c r="W81" s="27"/>
+      <c r="X81" s="27"/>
+      <c r="Y81" s="27"/>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A82" s="18">
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>624</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>609</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F82" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD03)CSDMtrTemp-Mon</v>
+      </c>
+      <c r="G82" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H82" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I82" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J82" s="24" t="s">
+        <v>628</v>
+      </c>
+      <c r="K82" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L82" s="24">
+        <v>1</v>
+      </c>
+      <c r="M82" s="27"/>
+      <c r="N82" s="27"/>
+      <c r="O82" s="27"/>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="27"/>
+      <c r="R82" s="27"/>
+      <c r="S82" s="27"/>
+      <c r="T82" s="27"/>
+      <c r="U82" s="27"/>
+      <c r="V82" s="27"/>
+      <c r="W82" s="27"/>
+      <c r="X82" s="27"/>
+      <c r="Y82" s="27"/>
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A83" s="18">
+        <v>82</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="E83" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F83" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>$(PREFIX_MOD03)CSEMtrTemp-Mon</v>
+      </c>
+      <c r="G83" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I83" s="24" t="s">
+        <v>604</v>
+      </c>
+      <c r="J83" s="24" t="s">
+        <v>629</v>
+      </c>
+      <c r="K83" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="L83" s="24">
+        <v>1</v>
+      </c>
+      <c r="M83" s="27"/>
+      <c r="N83" s="27"/>
+      <c r="O83" s="27"/>
+      <c r="P83" s="27"/>
+      <c r="Q83" s="27"/>
+      <c r="R83" s="27"/>
+      <c r="S83" s="27"/>
+      <c r="T83" s="27"/>
+      <c r="U83" s="27"/>
+      <c r="V83" s="27"/>
+      <c r="W83" s="27"/>
+      <c r="X83" s="27"/>
+      <c r="Y83" s="27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B18:B32">
@@ -16282,7 +16994,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E79" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E83" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"-Mon,-Sel,-Sts,-SP,-RB,-Cmd"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>